<commit_message>
Added tasks and Assignments.  Added updates to est. and actual
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Very High</t>
   </si>
@@ -188,6 +188,21 @@
   </si>
   <si>
     <t>Decimal format for seconds only field 0.1</t>
+  </si>
+  <si>
+    <t>Set user input length for all textfields.</t>
+  </si>
+  <si>
+    <t>Consider taking the existing combobox for Pace out.  This will have to refactor some code but may be beneficial in long???</t>
+  </si>
+  <si>
+    <t>Junit test for the Unit Converter class.</t>
+  </si>
+  <si>
+    <t>Update UI layout to compensate for textfields that were taken out.</t>
+  </si>
+  <si>
+    <t>Misc UI updates to enhance layout visually??</t>
   </si>
 </sst>
 </file>
@@ -316,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -363,6 +378,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,11 +599,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="290673040"/>
-        <c:axId val="290665984"/>
+        <c:axId val="518877680"/>
+        <c:axId val="518879856"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="290673040"/>
+        <c:axId val="518877680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,14 +646,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290665984"/>
+        <c:crossAx val="518879856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="290665984"/>
+        <c:axId val="518879856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +704,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290673040"/>
+        <c:crossAx val="518877680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -959,11 +983,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292170640"/>
-        <c:axId val="292176520"/>
+        <c:axId val="518874960"/>
+        <c:axId val="517913088"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="292170640"/>
+        <c:axId val="518874960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1033,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1076,14 +1099,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292176520"/>
+        <c:crossAx val="517913088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="292176520"/>
+        <c:axId val="517913088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +1157,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1201,7 +1223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292170640"/>
+        <c:crossAx val="518874960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2706,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,8 +2784,12 @@
       <c r="C4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -2773,8 +2799,15 @@
       <c r="C5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
@@ -2784,8 +2817,15 @@
       <c r="C6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -2795,8 +2835,12 @@
       <c r="C7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
@@ -2806,8 +2850,12 @@
       <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
@@ -2817,8 +2865,15 @@
       <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
@@ -2828,8 +2883,12 @@
       <c r="C10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
@@ -2841,8 +2900,12 @@
       <c r="C11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -2857,7 +2920,9 @@
       <c r="D12" s="9">
         <v>3</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -2872,7 +2937,9 @@
       <c r="D13" s="9">
         <v>3</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" t="s">
         <v>54</v>
       </c>
@@ -2887,7 +2954,9 @@
       <c r="D14" s="14">
         <v>3</v>
       </c>
-      <c r="E14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
@@ -2899,8 +2968,12 @@
       <c r="C15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="G15" t="s">
         <v>47</v>
       </c>
@@ -2915,8 +2988,15 @@
       <c r="C16" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0.1</v>
+      </c>
       <c r="G16" t="s">
         <v>46</v>
       </c>
@@ -2931,8 +3011,15 @@
       <c r="C17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="13"/>
+      <c r="D17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
@@ -2941,21 +3028,39 @@
       <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0.5</v>
+      </c>
       <c r="G18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>4</v>
       </c>
       <c r="B19" s="13">
         <v>16</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="13"/>
+      <c r="C19" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="25"/>
       <c r="G19" t="s">
         <v>49</v>
       </c>
@@ -2964,50 +3069,97 @@
       <c r="B20" s="13">
         <v>17</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="14">
+        <v>2</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="C21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2</v>
+      </c>
+      <c r="E21" s="9"/>
       <c r="G21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="13">
-        <f>SUM(D4:D21)</f>
-        <v>9</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="G22" t="s">
+      <c r="D27" s="13">
+        <f>SUM(D4:D22)</f>
+        <v>34.5</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="G27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added item to remove console output
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9975" windowHeight="5505"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="4" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Burndown Chart" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
   <si>
     <t>Very High</t>
   </si>
@@ -227,6 +228,9 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>Remove console output</t>
   </si>
 </sst>
 </file>
@@ -643,11 +647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289315832"/>
-        <c:axId val="289315048"/>
+        <c:axId val="264037400"/>
+        <c:axId val="264029952"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="289315832"/>
+        <c:axId val="264037400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,7 +697,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -760,14 +763,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289315048"/>
+        <c:crossAx val="264029952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="289315048"/>
+        <c:axId val="264029952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +821,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -885,7 +887,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289315832"/>
+        <c:crossAx val="264037400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1809,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,42 +2335,58 @@
       </c>
       <c r="G27" s="26"/>
     </row>
-    <row r="28" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="13">
+        <v>23</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="F28" s="13"/>
       <c r="G28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="23"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="13">
-        <f>SUM(D4:D28)</f>
-        <v>36</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13">
-        <f>SUM(F4:F28)</f>
+      <c r="D30" s="13">
+        <f>SUM(D4:D29)</f>
+        <v>36.25</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13">
+        <f>SUM(F4:F29)</f>
         <v>14.899999999999999</v>
       </c>
-      <c r="G29" s="26"/>
-      <c r="H29">
-        <f>D29-F29</f>
-        <v>21.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
       <c r="G30" s="26"/>
+      <c r="H30">
+        <f>D30-F30</f>
+        <v>21.35</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32" s="13"/>
@@ -2384,6 +2402,9 @@
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2772,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2811,7 +2832,7 @@
         <v>42677</v>
       </c>
       <c r="B3" s="20">
-        <f t="shared" ref="B3:B18" si="0">B2-C3</f>
+        <f t="shared" ref="B3:B8" si="0">B2-C3</f>
         <v>29</v>
       </c>
       <c r="C3" s="9">

</xml_diff>

<commit_message>
Daily Scrum and backlog update
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 2 Backlog.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Burndown Chart" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -647,11 +646,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="264037400"/>
-        <c:axId val="264029952"/>
+        <c:axId val="302343600"/>
+        <c:axId val="302343992"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="264037400"/>
+        <c:axId val="302343600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,14 +762,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264029952"/>
+        <c:crossAx val="302343992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="264029952"/>
+        <c:axId val="302343992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,7 +886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264037400"/>
+        <c:crossAx val="302343600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1813,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>